<commit_message>
Changes Made in Profile.cs
</commit_message>
<xml_diff>
--- a/User_Details.xlsx
+++ b/User_Details.xlsx
@@ -8,22 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ADVANCED TASKS\NunitTask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49058CBC-D2C8-4CCE-843A-C980AB742152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647B70C7-9B72-40C1-A334-4CF45D3B4833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11025" yWindow="-13620" windowWidth="24240" windowHeight="13140" activeTab="5" xr2:uid="{5BF696D1-3630-4D1F-95DB-5B6DC96DAECF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="11" xr2:uid="{5BF696D1-3630-4D1F-95DB-5B6DC96DAECF}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="1" r:id="rId1"/>
     <sheet name="SignIn" sheetId="2" r:id="rId2"/>
-    <sheet name="ManageListings" sheetId="3" r:id="rId3"/>
-    <sheet name="Time" sheetId="4" r:id="rId4"/>
-    <sheet name="ShareSkillDetails" sheetId="6" r:id="rId5"/>
-    <sheet name="ProfileAvailability" sheetId="7" r:id="rId6"/>
-    <sheet name="Language" sheetId="8" r:id="rId7"/>
-    <sheet name="Skills" sheetId="9" r:id="rId8"/>
-    <sheet name="Education" sheetId="10" r:id="rId9"/>
-    <sheet name="Certification" sheetId="12" r:id="rId10"/>
-    <sheet name="Description" sheetId="13" r:id="rId11"/>
+    <sheet name="UpdateLanguage" sheetId="16" r:id="rId3"/>
+    <sheet name="ManageListings" sheetId="3" r:id="rId4"/>
+    <sheet name="Time" sheetId="4" r:id="rId5"/>
+    <sheet name="ShareSkillDetails" sheetId="6" r:id="rId6"/>
+    <sheet name="AvailabilityTime" sheetId="7" r:id="rId7"/>
+    <sheet name="AvailabilityHour" sheetId="14" r:id="rId8"/>
+    <sheet name="AvailabilitySalary" sheetId="15" r:id="rId9"/>
+    <sheet name="Language" sheetId="8" r:id="rId10"/>
+    <sheet name="Skills" sheetId="9" r:id="rId11"/>
+    <sheet name="Education" sheetId="10" r:id="rId12"/>
+    <sheet name="Certification" sheetId="12" r:id="rId13"/>
+    <sheet name="Description" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="85">
   <si>
     <t>FirstName</t>
   </si>
@@ -187,12 +190,6 @@
     <t>Hours</t>
   </si>
   <si>
-    <t>As needed</t>
-  </si>
-  <si>
-    <t>More than $1000 per month</t>
-  </si>
-  <si>
     <t>Salary</t>
   </si>
   <si>
@@ -256,7 +253,46 @@
     <t>Udemy</t>
   </si>
   <si>
-    <t>Nunit Testing description ongoing. Test, test, test!</t>
+    <t>Full Time</t>
+  </si>
+  <si>
+    <t>Nunit Testing description ongoing. Test, test, test! Advanced task, automation test!</t>
+  </si>
+  <si>
+    <t>change@1234</t>
+  </si>
+  <si>
+    <t>More than 30hours a week</t>
+  </si>
+  <si>
+    <t>Between $500 and $1000 per month</t>
+  </si>
+  <si>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>UpdatedLanguage</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Expert</t>
+  </si>
+  <si>
+    <t>Selenium/C#</t>
+  </si>
+  <si>
+    <t>Information Technology</t>
+  </si>
+  <si>
+    <t>University of San Carlos</t>
+  </si>
+  <si>
+    <t>PHD</t>
   </si>
 </sst>
 </file>
@@ -267,7 +303,7 @@
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +315,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -305,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -320,6 +362,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -695,6 +740,164 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CFBC00-2E17-4D1B-B094-3E2FB3042CC7}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9E7EE9-CA6D-4DA1-A490-E299393BFD3B}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45A93FB-7016-4333-8F2B-7342067E80D7}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4">
+        <v>2007</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF91B35-16FF-41E6-8DE3-B257D75C762F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -711,21 +914,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
         <v>68</v>
-      </c>
-      <c r="B1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>2021</v>
@@ -736,12 +939,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128EBF35-795D-4735-A370-57FE2A1BABC5}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,9 +957,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>73</v>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -766,44 +969,96 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BFFE781-02AA-436F-95F8-FDDE450A399A}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{18B4F844-9273-412B-826D-F9ACDD3F0BD0}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{8B759284-4A1E-49C7-9DEA-4B9D589DF067}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{2CE4E126-1F62-4527-8B9A-639A57BC8CE4}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{DD4E173B-A957-44BA-9176-039286FE68AE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30332AAA-850F-4C42-A703-2F672F7BFAE0}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>46</v>
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{18B4F844-9273-412B-826D-F9ACDD3F0BD0}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{8B759284-4A1E-49C7-9DEA-4B9D589DF067}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA6FE23-F463-4F5D-B37F-DBEAAACC6D76}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -901,7 +1156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6277BEF2-B76A-48D0-8C51-FEEE085740C1}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -1024,7 +1279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81BD2281-4BA2-409B-A4A0-026AF71DC7C4}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -1123,12 +1378,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50ABABE1-D2F2-4752-B0C6-9F9C43012D19}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,26 +1393,14 @@
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1165,122 +1408,64 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CFBC00-2E17-4D1B-B094-3E2FB3042CC7}">
-  <dimension ref="A1:B2"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61368459-1752-4BE3-A97A-64179B8BF41B}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B9:B10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9E7EE9-CA6D-4DA1-A490-E299393BFD3B}">
-  <dimension ref="A1:B2"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8D8883-8B84-4332-9A7F-0F3BA711328C}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45A93FB-7016-4333-8F2B-7342067E80D7}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2">
-        <v>2006</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>